<commit_message>
added excel utility and ddt scenario with excel file
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duotech\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duotech\eclipsez\cucumber-bdd-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F160C742-F009-4573-9670-B83E0C5141A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AFB377-A13D-49AE-A9C9-01A75D4B672F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
+    <workbookView xWindow="4908" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Execute</t>
   </si>
@@ -99,28 +99,35 @@
     <t>$26.00</t>
   </si>
   <si>
-    <t>$28.98</t>
-  </si>
-  <si>
-    <t>$17.40</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>Faded Short Sleeve T-shirts</t>
   </si>
   <si>
-    <t>passed</t>
-  </si>
-  <si>
-    <t>fail</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>$16.40</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>$28.99</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,12 +482,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752E530-4C12-4F61-B562-BFFFB21CE8A8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -511,7 +520,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
@@ -531,7 +540,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -549,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -577,13 +586,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -595,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -606,7 +615,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -618,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>